<commit_message>
Week 2, Day 2 - start
</commit_message>
<xml_diff>
--- a/week2/day1/statistics.xlsx
+++ b/week2/day1/statistics.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
@@ -24,11 +33,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -39,8 +48,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -55,31 +101,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,13 +116,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -109,14 +124,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -139,8 +146,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,7 +170,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,21 +178,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,19 +201,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -216,55 +339,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,103 +381,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,11 +460,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,9 +484,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,13 +497,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -506,130 +515,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -640,7 +649,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -816,7 +825,7 @@
                   <c:v>0.631944444444444</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.630555555555556</c:v>
+                  <c:v>0.644444444444444</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.618055555555556</c:v>
@@ -1902,13 +1911,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:A18"/>
+  <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="12.8888888888889"/>
   </cols>
@@ -1918,86 +1927,128 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>0.631944444444444</v>
       </c>
+      <c r="D3" s="1">
+        <v>0.618055555555556</v>
+      </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>0.625</v>
       </c>
+      <c r="D4" s="1">
+        <v>0.625</v>
+      </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>0.628472222222222</v>
       </c>
+      <c r="D5" s="1">
+        <v>0.628472222222222</v>
+      </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>0.635416666666667</v>
       </c>
+      <c r="D6" s="1">
+        <v>0.630555555555556</v>
+      </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>0.633333333333333</v>
       </c>
+      <c r="D7" s="1">
+        <v>0.631944444444444</v>
+      </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>0.645833333333333</v>
       </c>
+      <c r="D8" s="1">
+        <v>0.631944444444444</v>
+      </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>0.639583333333333</v>
       </c>
+      <c r="D9" s="1">
+        <v>0.631944444444444</v>
+      </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>0.631944444444444</v>
       </c>
+      <c r="D10" s="1">
+        <v>0.633333333333333</v>
+      </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>0.631944444444444</v>
       </c>
+      <c r="D11" s="1">
+        <v>0.635416666666667</v>
+      </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>0.630555555555556</v>
+        <v>0.644444444444444</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.639583333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>0.618055555555556</v>
       </c>
+      <c r="D13" s="1">
+        <v>0.645833333333333</v>
+      </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <f>AVERAGE(A3:A13)</f>
-        <v>0.632007575757576</v>
+        <v>0.633270202020202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <f>MEDIAN(A3:A13)</f>
         <v>0.631944444444444</v>
       </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <f>MODE(A3:A13)</f>
         <v>0.631944444444444</v>
       </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="2">
-        <f>STDEV(A3:A13)</f>
-        <v>0.00721323255591582</v>
-      </c>
+      <c r="A18" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="D3:D13">
+    <sortCondition ref="D3"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>